<commit_message>
update another page of blog entries
</commit_message>
<xml_diff>
--- a/Work In Progress.xlsx
+++ b/Work In Progress.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\PS7 Scripting Guy blog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\PSScriptingBlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8271D100-E7E0-4CC0-B790-F9656E91AEA6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D04BDE-264A-41BE-A89E-BC959AE68A21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31785" yWindow="1905" windowWidth="23040" windowHeight="12735" xr2:uid="{AA304ACB-70A8-4EB0-A065-620CD9357C65}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{AA304ACB-70A8-4EB0-A065-620CD9357C65}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="156">
   <si>
     <t>Date</t>
   </si>
@@ -276,9 +276,6 @@
     <t>Drafted</t>
   </si>
   <si>
-    <t>Next</t>
-  </si>
-  <si>
     <t>How Do I Bind to a User Account in a Sub-OU?</t>
   </si>
   <si>
@@ -459,7 +456,43 @@
     <t>https://devblogs.microsoft.com/scripting/how-can-i-determine-if-my-users-have-certain-files-on-their-computers/</t>
   </si>
   <si>
-    <t>https://devblogs.microsoft.com/scripting/page/1077/</t>
+    <t>How Can I Change a User’s Password?</t>
+  </si>
+  <si>
+    <t>https://devblogs.microsoft.com/scripting/how-can-i-change-a-users-password/</t>
+  </si>
+  <si>
+    <t>How Can I Pick Out and Save Specific Lines in a Text File?</t>
+  </si>
+  <si>
+    <t>https://devblogs.microsoft.com/scripting/how-can-i-pick-out-and-save-specific-lines-in-a-text-file/</t>
+  </si>
+  <si>
+    <t>How Can I Change a Read-only File to a Read-write File?</t>
+  </si>
+  <si>
+    <t>https://devblogs.microsoft.com/scripting/how-can-i-change-a-read-only-file-to-a-read-write-file/</t>
+  </si>
+  <si>
+    <t>How Can I Get a List of All the Files in a Folder and Its Subfolders?</t>
+  </si>
+  <si>
+    <t>https://devblogs.microsoft.com/scripting/how-can-i-get-a-list-of-all-the-files-in-a-folder-and-its-subfolders/</t>
+  </si>
+  <si>
+    <t>How Can I Determine the OU a User Account Belongs To?</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>https://devblogs.microsoft.com/scripting/how-can-i-determine-the-ou-a-user-account-belongs-to/</t>
+  </si>
+  <si>
+    <t>https://devblogs.microsoft.com/scripting/page/1076/</t>
+  </si>
+  <si>
+    <t>Next page</t>
   </si>
 </sst>
 </file>
@@ -850,10 +883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8BF330-BB8A-4A7D-B013-2E21A0FB91FA}">
-  <dimension ref="A1:J70"/>
+  <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,7 +1056,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E7" t="s">
         <v>16</v>
@@ -1069,7 +1102,7 @@
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F9" t="s">
         <v>26</v>
@@ -1092,7 +1125,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E10" t="s">
         <v>16</v>
@@ -1278,7 +1311,7 @@
         <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F19" t="s">
         <v>55</v>
@@ -1581,16 +1614,16 @@
         <v>38247</v>
       </c>
       <c r="B34" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" t="s">
         <v>84</v>
       </c>
-      <c r="C34" t="s">
+      <c r="E34" t="s">
         <v>85</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>87</v>
       </c>
       <c r="H34">
         <v>1081</v>
@@ -1601,16 +1634,16 @@
         <v>38250</v>
       </c>
       <c r="B35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="C35" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" t="s">
-        <v>16</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="H35">
         <v>1081</v>
@@ -1621,7 +1654,7 @@
         <v>38251</v>
       </c>
       <c r="B36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C36" t="s">
         <v>9</v>
@@ -1630,13 +1663,13 @@
         <v>16</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H36">
         <v>1081</v>
       </c>
       <c r="J36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -1644,22 +1677,22 @@
         <v>38252</v>
       </c>
       <c r="B37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
       </c>
       <c r="E37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H37">
         <v>1081</v>
       </c>
       <c r="J37" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -1667,16 +1700,16 @@
         <v>38253</v>
       </c>
       <c r="B38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
       </c>
       <c r="E38" t="s">
-        <v>86</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>102</v>
+        <v>85</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="H38">
         <v>1081</v>
@@ -1687,22 +1720,22 @@
         <v>38254</v>
       </c>
       <c r="B39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C39" t="s">
         <v>5</v>
       </c>
       <c r="E39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H39">
         <v>1080</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -1710,16 +1743,16 @@
         <v>38257</v>
       </c>
       <c r="B40" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" t="s">
+        <v>16</v>
+      </c>
+      <c r="F40" t="s">
         <v>108</v>
-      </c>
-      <c r="C40" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" t="s">
-        <v>16</v>
-      </c>
-      <c r="F40" t="s">
-        <v>109</v>
       </c>
       <c r="H40">
         <v>1080</v>
@@ -1731,16 +1764,16 @@
         <v>38258</v>
       </c>
       <c r="B41" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" t="s">
+        <v>16</v>
+      </c>
+      <c r="F41" t="s">
         <v>110</v>
-      </c>
-      <c r="C41" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" t="s">
-        <v>16</v>
-      </c>
-      <c r="F41" t="s">
-        <v>111</v>
       </c>
       <c r="H41">
         <v>1080</v>
@@ -1752,16 +1785,16 @@
         <v>38259</v>
       </c>
       <c r="B42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C42" t="s">
         <v>5</v>
       </c>
       <c r="E42" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H42">
         <v>1080</v>
@@ -1773,16 +1806,16 @@
         <v>38260</v>
       </c>
       <c r="B43" t="s">
+        <v>113</v>
+      </c>
+      <c r="C43" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" t="s">
         <v>114</v>
-      </c>
-      <c r="C43" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" t="s">
-        <v>16</v>
-      </c>
-      <c r="F43" t="s">
-        <v>115</v>
       </c>
       <c r="H43">
         <v>1080</v>
@@ -1794,16 +1827,16 @@
         <v>38261</v>
       </c>
       <c r="B44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C44" t="s">
         <v>5</v>
       </c>
       <c r="E44" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F44" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H44">
         <v>1079</v>
@@ -1815,7 +1848,7 @@
         <v>38264</v>
       </c>
       <c r="B45" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C45" t="s">
         <v>9</v>
@@ -1824,7 +1857,7 @@
         <v>16</v>
       </c>
       <c r="F45" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H45">
         <v>1079</v>
@@ -1836,7 +1869,7 @@
         <v>38265</v>
       </c>
       <c r="B46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C46" t="s">
         <v>9</v>
@@ -1845,7 +1878,7 @@
         <v>16</v>
       </c>
       <c r="F46" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H46">
         <v>1079</v>
@@ -1857,16 +1890,16 @@
         <v>38266</v>
       </c>
       <c r="B47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C47" t="s">
         <v>5</v>
       </c>
       <c r="E47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H47">
         <v>1079</v>
@@ -1878,7 +1911,7 @@
         <v>38267</v>
       </c>
       <c r="B48" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C48" t="s">
         <v>9</v>
@@ -1887,7 +1920,7 @@
         <v>16</v>
       </c>
       <c r="F48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H48">
         <v>1079</v>
@@ -1899,16 +1932,16 @@
         <v>38268</v>
       </c>
       <c r="B49" t="s">
+        <v>132</v>
+      </c>
+      <c r="C49" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" t="s">
+        <v>16</v>
+      </c>
+      <c r="F49" t="s">
         <v>133</v>
-      </c>
-      <c r="C49" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" t="s">
-        <v>16</v>
-      </c>
-      <c r="F49" t="s">
-        <v>134</v>
       </c>
       <c r="H49">
         <v>1078</v>
@@ -1920,22 +1953,22 @@
         <v>38271</v>
       </c>
       <c r="B50" t="s">
+        <v>134</v>
+      </c>
+      <c r="C50" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" t="s">
+        <v>16</v>
+      </c>
+      <c r="F50" t="s">
         <v>135</v>
-      </c>
-      <c r="C50" t="s">
-        <v>9</v>
-      </c>
-      <c r="E50" t="s">
-        <v>16</v>
-      </c>
-      <c r="F50" t="s">
-        <v>136</v>
       </c>
       <c r="H50">
         <v>1078</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -1943,16 +1976,16 @@
         <v>38272</v>
       </c>
       <c r="B51" t="s">
+        <v>137</v>
+      </c>
+      <c r="C51" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" t="s">
         <v>138</v>
-      </c>
-      <c r="C51" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" t="s">
-        <v>16</v>
-      </c>
-      <c r="F51" t="s">
-        <v>139</v>
       </c>
       <c r="H51">
         <v>1078</v>
@@ -1964,16 +1997,16 @@
         <v>38273</v>
       </c>
       <c r="B52" t="s">
+        <v>139</v>
+      </c>
+      <c r="C52" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" s="5" t="s">
         <v>140</v>
-      </c>
-      <c r="C52" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" t="s">
-        <v>16</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="H52">
         <v>1078</v>
@@ -1985,13 +2018,16 @@
         <v>38274</v>
       </c>
       <c r="B53" t="s">
+        <v>141</v>
+      </c>
+      <c r="C53" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" t="s">
+        <v>16</v>
+      </c>
+      <c r="F53" t="s">
         <v>142</v>
-      </c>
-      <c r="E53" t="s">
-        <v>16</v>
-      </c>
-      <c r="F53" t="s">
-        <v>143</v>
       </c>
       <c r="H53">
         <v>1078</v>
@@ -1999,98 +2035,201 @@
       <c r="J53" s="3"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="2"/>
+      <c r="A54" s="2">
+        <v>38275</v>
+      </c>
+      <c r="B54" t="s">
+        <v>143</v>
+      </c>
+      <c r="C54" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54" t="s">
+        <v>85</v>
+      </c>
+      <c r="F54" t="s">
+        <v>144</v>
+      </c>
+      <c r="H54">
+        <v>1077</v>
+      </c>
       <c r="J54" s="3"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="2"/>
+      <c r="A55" s="2">
+        <v>38278</v>
+      </c>
+      <c r="B55" t="s">
+        <v>145</v>
+      </c>
+      <c r="C55" t="s">
+        <v>84</v>
+      </c>
+      <c r="E55" t="s">
+        <v>85</v>
+      </c>
+      <c r="F55" t="s">
+        <v>146</v>
+      </c>
+      <c r="H55">
+        <v>1077</v>
+      </c>
       <c r="J55" s="3"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>83</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>144</v>
+      <c r="A56" s="2">
+        <v>38279</v>
+      </c>
+      <c r="B56" t="s">
+        <v>147</v>
+      </c>
+      <c r="C56" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" t="s">
+        <v>16</v>
+      </c>
+      <c r="F56" t="s">
+        <v>148</v>
+      </c>
+      <c r="H56">
+        <v>1077</v>
       </c>
       <c r="J56" s="3"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="2"/>
+      <c r="A57" s="2">
+        <v>38280</v>
+      </c>
+      <c r="B57" t="s">
+        <v>149</v>
+      </c>
+      <c r="C57" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" t="s">
+        <v>16</v>
+      </c>
+      <c r="F57" t="s">
+        <v>150</v>
+      </c>
+      <c r="H57">
+        <v>1077</v>
+      </c>
       <c r="J57" s="3"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>117</v>
+      <c r="A58" s="2">
+        <v>38281</v>
+      </c>
+      <c r="B58" t="s">
+        <v>151</v>
+      </c>
+      <c r="C58" t="s">
+        <v>152</v>
+      </c>
+      <c r="E58" t="s">
+        <v>16</v>
+      </c>
+      <c r="F58" t="s">
+        <v>153</v>
+      </c>
+      <c r="H58">
+        <v>1077</v>
       </c>
       <c r="J58" s="3"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
-      <c r="B59" t="s">
+      <c r="J59" s="3"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+      <c r="J60" s="3"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>155</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="J61" s="3"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+      <c r="J62" s="3"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="J63" s="3"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="2"/>
+      <c r="B64" t="s">
+        <v>117</v>
+      </c>
+      <c r="D64" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="E64" t="s">
         <v>119</v>
       </c>
-      <c r="E59" t="s">
-        <v>120</v>
-      </c>
-      <c r="J59" s="3"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="2">
+      <c r="J64" s="3"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
         <v>40616</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B70" t="s">
+        <v>92</v>
+      </c>
+      <c r="C70" t="s">
+        <v>9</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E70" t="s">
         <v>93</v>
       </c>
-      <c r="C65" t="s">
-        <v>9</v>
-      </c>
-      <c r="D65" s="4" t="s">
+      <c r="F70" t="s">
+        <v>91</v>
+      </c>
+      <c r="I70" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>96</v>
       </c>
-      <c r="E65" t="s">
-        <v>94</v>
-      </c>
-      <c r="F65" t="s">
-        <v>92</v>
-      </c>
-      <c r="I65" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
+      <c r="F75" t="s">
         <v>98</v>
-      </c>
-      <c r="F70" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B56" r:id="rId1" xr:uid="{DACACF0A-FB32-419D-BC67-69B436368D1F}"/>
+    <hyperlink ref="B61" r:id="rId1" xr:uid="{DACACF0A-FB32-419D-BC67-69B436368D1F}"/>
     <hyperlink ref="J39" r:id="rId2" xr:uid="{11E95735-87F4-4DC8-BFD5-8872799C8690}"/>
-    <hyperlink ref="F38" r:id="rId3" xr:uid="{7D0AA1CD-01E6-4032-B90F-A070702BF03D}"/>
-    <hyperlink ref="F3" r:id="rId4" xr:uid="{8CE6B5D9-C7A8-4A69-82E8-437815864D04}"/>
-    <hyperlink ref="F5" r:id="rId5" xr:uid="{D29FDDD4-B72A-452C-A85D-30D9FD56A3BA}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{D3297172-9820-401F-93CA-1C48D7F57A1A}"/>
-    <hyperlink ref="F10" r:id="rId7" xr:uid="{332DEB36-8511-4409-AC90-793E3D010258}"/>
-    <hyperlink ref="F52" r:id="rId8" xr:uid="{063CECB2-190C-41F5-9F52-881696E8B586}"/>
+    <hyperlink ref="F3" r:id="rId3" xr:uid="{8CE6B5D9-C7A8-4A69-82E8-437815864D04}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{D29FDDD4-B72A-452C-A85D-30D9FD56A3BA}"/>
+    <hyperlink ref="F7" r:id="rId5" xr:uid="{D3297172-9820-401F-93CA-1C48D7F57A1A}"/>
+    <hyperlink ref="F10" r:id="rId6" xr:uid="{332DEB36-8511-4409-AC90-793E3D010258}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>